<commit_message>
Update scale factors and planet data
</commit_message>
<xml_diff>
--- a/ScaleConversions.xlsx
+++ b/ScaleConversions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsmall/Git/lassp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A43BCC-3AFF-AF44-A1A0-05F853C9A966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C96CAA-69FD-354E-BFD4-B88933B7AC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19540" yWindow="1900" windowWidth="10000" windowHeight="9680" activeTab="3" xr2:uid="{26327C24-766D-5D49-9BFD-19571218BEE3}"/>
+    <workbookView xWindow="8320" yWindow="1900" windowWidth="24260" windowHeight="15880" xr2:uid="{26327C24-766D-5D49-9BFD-19571218BEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Factors" sheetId="1" r:id="rId1"/>
@@ -111,10 +111,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="#,##0.000000000000000000000000000000"/>
     <numFmt numFmtId="170" formatCode="0.000000000000000000000000000000"/>
+    <numFmt numFmtId="172" formatCode="0_);\(0\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -169,9 +170,9 @@
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -489,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{411FE549-8177-1648-BB72-D66602C113A9}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,18 +525,18 @@
         <v>14</v>
       </c>
       <c r="B2" s="2">
-        <v>491</v>
+        <v>447</v>
       </c>
       <c r="C2" s="2">
         <f>B2/5280</f>
-        <v>9.2992424242424238E-2</v>
+        <v>8.4659090909090906E-2</v>
       </c>
       <c r="D2" s="2">
-        <v>865370</v>
+        <v>864948</v>
       </c>
       <c r="E2" s="6">
         <f>C2/D2</f>
-        <v>1.0745972733330741E-7</v>
+        <v>9.7877665373052382E-8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -550,11 +551,11 @@
         <v>1</v>
       </c>
       <c r="D3" s="2">
-        <v>865370</v>
+        <v>864948</v>
       </c>
       <c r="E3" s="6">
         <f>C3/D3</f>
-        <v>1.1555750719345483E-6</v>
+        <v>1.1561388661514912E-6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -562,15 +563,15 @@
         <v>15</v>
       </c>
       <c r="B4" s="2">
-        <f>865370*5280</f>
-        <v>4569153600</v>
+        <f>D4*5280</f>
+        <v>4566925440</v>
       </c>
       <c r="C4" s="2">
         <f>B4/5280</f>
-        <v>865370</v>
+        <v>864948</v>
       </c>
       <c r="D4" s="2">
-        <v>865370</v>
+        <v>864948</v>
       </c>
       <c r="E4" s="6">
         <f>C4/D4</f>
@@ -582,18 +583,18 @@
         <v>16</v>
       </c>
       <c r="B5" s="2">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="2">
         <f>B5/5280</f>
-        <v>1.6098484848484848E-2</v>
+        <v>1.571969696969697E-2</v>
       </c>
       <c r="D5" s="2">
-        <v>865370</v>
+        <v>864948</v>
       </c>
       <c r="E5" s="6">
         <f>C5/D5</f>
-        <v>1.8603007786825114E-8</v>
+        <v>1.8174152630790488E-8</v>
       </c>
     </row>
   </sheetData>
@@ -606,24 +607,23 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.6640625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
     </row>
@@ -631,130 +631,130 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="9">
         <f>LA!B2/Factors!$E$5</f>
-        <v>27952469.08235294</v>
-      </c>
-      <c r="C2" s="7">
+        <v>28612062.997590359</v>
+      </c>
+      <c r="C2" s="9">
         <f>LA!C2/Factors!$E$5</f>
-        <v>42466251.105882354</v>
+        <v>43468326.477108434</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="9">
         <f>LA!B3/Factors!$E$5</f>
-        <v>65043245.364705876</v>
-      </c>
-      <c r="C3" s="7">
+        <v>66578069.667469874</v>
+      </c>
+      <c r="C3" s="9">
         <f>LA!C3/Factors!$E$5</f>
-        <v>66118340.32941176</v>
+        <v>67678533.628915653</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="9">
         <f>LA!B4/Factors!$E$5</f>
-        <v>89232882.070588231</v>
-      </c>
-      <c r="C4" s="7">
+        <v>91338508.799999982</v>
+      </c>
+      <c r="C4" s="9">
         <f>LA!C4/Factors!$E$5</f>
-        <v>91920619.482352942</v>
+        <v>94089668.703614444</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="9">
         <f>LA!B5/Factors!$E$5</f>
-        <v>125248563.38823529</v>
-      </c>
-      <c r="C5" s="7">
+        <v>128204051.50843373</v>
+      </c>
+      <c r="C5" s="9">
         <f>LA!C5/Factors!$E$5</f>
-        <v>151050842.54117647</v>
+        <v>154615186.58313251</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="9">
         <f>LA!B6/Factors!$E$5</f>
-        <v>160726697.22352943</v>
-      </c>
-      <c r="C6" s="7">
+        <v>164519362.23614457</v>
+      </c>
+      <c r="C6" s="9">
         <f>LA!C6/Factors!$E$5</f>
-        <v>349943411.01176471</v>
+        <v>358201019.45060235</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="9">
         <f>LA!B7/Factors!$E$5</f>
-        <v>448852147.76470584</v>
-      </c>
-      <c r="C7" s="7">
+        <v>459443703.9036144</v>
+      </c>
+      <c r="C7" s="9">
         <f>LA!C7/Factors!$E$5</f>
-        <v>494543683.76470584</v>
+        <v>506213422.26506013</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="9">
         <f>LA!B8/Factors!$E$5</f>
-        <v>817609720.65882349</v>
-      </c>
-      <c r="C8" s="7">
+        <v>836902842.67951798</v>
+      </c>
+      <c r="C8" s="9">
         <f>LA!C8/Factors!$E$5</f>
-        <v>911142982.58823526</v>
+        <v>932643207.32530105</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="9">
         <f>LA!B9/Factors!$E$5</f>
-        <v>1661021720.4705882</v>
-      </c>
-      <c r="C9" s="7">
+        <v>1700216820.4337347</v>
+      </c>
+      <c r="C9" s="9">
         <f>LA!C9/Factors!$E$5</f>
-        <v>1819598227.7647059</v>
+        <v>1862535254.7469878</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="9">
         <f>LA!B10/Factors!$E$5</f>
-        <v>2692575339.1058826</v>
-      </c>
-      <c r="C10" s="7">
+        <v>2756111991.4409637</v>
+      </c>
+      <c r="C10" s="9">
         <f>LA!C10/Factors!$E$5</f>
-        <v>2753855752.0941172</v>
+        <v>2818838437.2433729</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="9">
         <f>LA!B11/Factors!$E$5</f>
-        <v>2753855752.0941172</v>
-      </c>
-      <c r="C11" s="7">
+        <v>2818838437.2433729</v>
+      </c>
+      <c r="C11" s="9">
         <f>LA!C11/Factors!$E$5</f>
-        <v>4468632220.7999992</v>
+        <v>4574078455.7493973</v>
       </c>
     </row>
   </sheetData>
@@ -907,7 +907,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86B68B4-F939-4D4E-BAA5-A0F71F38BFA3}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -920,10 +922,10 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -933,11 +935,11 @@
       </c>
       <c r="B2" s="1">
         <f>Factors!$E$2*Actual!B2</f>
-        <v>3.0037647058823524</v>
+        <v>2.8004819277108433</v>
       </c>
       <c r="C2" s="1">
         <f>Factors!$E$2*Actual!C2</f>
-        <v>4.5634117647058821</v>
+        <v>4.2545783132530124</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -946,11 +948,11 @@
       </c>
       <c r="B3" s="1">
         <f>Factors!$E$2*Actual!B3</f>
-        <v>6.9895294117647042</v>
+        <v>6.516506024096385</v>
       </c>
       <c r="C3" s="1">
         <f>Factors!$E$2*Actual!C3</f>
-        <v>7.1050588235294105</v>
+        <v>6.6242168674698787</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -959,11 +961,11 @@
       </c>
       <c r="B4" s="1">
         <f>Factors!$E$2*Actual!B4</f>
-        <v>9.5889411764705876</v>
+        <v>8.9399999999999977</v>
       </c>
       <c r="C4" s="1">
         <f>Factors!$E$2*Actual!C4</f>
-        <v>9.8777647058823526</v>
+        <v>9.2092771084337333</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -972,11 +974,11 @@
       </c>
       <c r="B5" s="1">
         <f>Factors!$E$2*Actual!B5</f>
-        <v>13.459176470588233</v>
+        <v>12.548313253012047</v>
       </c>
       <c r="C5" s="1">
         <f>Factors!$E$2*Actual!C5</f>
-        <v>16.231882352941174</v>
+        <v>15.133373493975901</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -985,11 +987,11 @@
       </c>
       <c r="B6" s="1">
         <f>Factors!$E$2*Actual!B6</f>
-        <v>17.271647058823529</v>
+        <v>16.102771084337348</v>
       </c>
       <c r="C6" s="1">
         <f>Factors!$E$2*Actual!C6</f>
-        <v>37.60482352941176</v>
+        <v>35.059879518072286</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -998,11 +1000,11 @@
       </c>
       <c r="B7" s="1">
         <f>Factors!$E$2*Actual!B7</f>
-        <v>48.2335294117647</v>
+        <v>44.969277108433729</v>
       </c>
       <c r="C7" s="1">
         <f>Factors!$E$2*Actual!C7</f>
-        <v>53.143529411764696</v>
+        <v>49.546987951807218</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1011,11 +1013,11 @@
       </c>
       <c r="B8" s="1">
         <f>Factors!$E$2*Actual!B8</f>
-        <v>87.860117647058814</v>
+        <v>81.914096385542166</v>
       </c>
       <c r="C8" s="1">
         <f>Factors!$E$2*Actual!C8</f>
-        <v>97.911176470588217</v>
+        <v>91.284939759036135</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1024,11 +1026,11 @@
       </c>
       <c r="B9" s="1">
         <f>Factors!$E$2*Actual!B9</f>
-        <v>178.49294117647057</v>
+        <v>166.41325301204816</v>
       </c>
       <c r="C9" s="1">
         <f>Factors!$E$2*Actual!C9</f>
-        <v>195.5335294117647</v>
+        <v>182.30060240963854</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1037,11 +1039,11 @@
       </c>
       <c r="B10" s="1">
         <f>Factors!$E$2*Actual!B10</f>
-        <v>289.34341176470588</v>
+        <v>269.76180722891564</v>
       </c>
       <c r="C10" s="1">
         <f>Factors!$E$2*Actual!C10</f>
-        <v>295.92858823529406</v>
+        <v>275.90132530120479</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1050,11 +1052,11 @@
       </c>
       <c r="B11" s="1">
         <f>Factors!$E$2*Actual!B11</f>
-        <v>295.92858823529406</v>
+        <v>275.90132530120479</v>
       </c>
       <c r="C11" s="1">
         <f>Factors!$E$2*Actual!C11</f>
-        <v>480.19799999999987</v>
+        <v>447.70012048192768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>